<commit_message>
28.10.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/September/Others/Sales target -Rajshahi-September,2020 - Feedback of Rajshahi Region.xlsx
+++ b/2020/September/Others/Sales target -Rajshahi-September,2020 - Feedback of Rajshahi Region.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saiful.islam\Desktop\Target September 2020\Target Split\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7455"/>
   </bookViews>
@@ -22,9 +17,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Distributor Primary'!$A$3:$AJ$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Distributor Secondary'!$A$3:$AJ$21</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -807,12 +802,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -937,7 +932,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -995,6 +990,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1103,39 +1104,39 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1144,14 +1145,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1168,10 +1169,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1191,7 +1192,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1205,7 +1206,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1215,11 +1216,11 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1231,10 +1232,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -1249,19 +1250,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1295,10 +1296,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1310,7 +1311,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="15" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1325,7 +1326,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1334,37 +1335,37 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="15" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="8" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
@@ -1420,7 +1421,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="4" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="4" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1430,23 +1431,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="18" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1487,6 +1477,32 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1817,7 +1833,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1852,7 +1868,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2029,24 +2045,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:AJ21"/>
+  <dimension ref="A1:AK24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="AH27" sqref="AH27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2055,32 +2071,33 @@
     <col min="2" max="2" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12" style="3" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="8.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="7.5703125" style="3" customWidth="1"/>
-    <col min="34" max="34" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="5" width="7.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="8.140625" style="3" customWidth="1"/>
+    <col min="11" max="13" width="8.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" style="3" customWidth="1"/>
+    <col min="17" max="20" width="8.5703125" style="3" customWidth="1"/>
+    <col min="21" max="22" width="8.140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="8.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="8.5703125" style="3" customWidth="1"/>
+    <col min="31" max="31" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" style="3" customWidth="1"/>
+    <col min="33" max="34" width="8.5703125" style="3" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" style="3" customWidth="1"/>
+    <col min="36" max="36" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15">
+    <row r="1" spans="1:36" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>248</v>
       </c>
@@ -2188,7 +2205,7 @@
       </c>
     </row>
     <row r="3" spans="1:36" s="10" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="141" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -3417,227 +3434,227 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="145" customFormat="1">
-      <c r="A14" s="141" t="s">
+    <row r="14" spans="1:36" s="159" customFormat="1">
+      <c r="A14" s="155" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="142" t="s">
+      <c r="B14" s="156" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="143">
+      <c r="C14" s="157">
         <f t="shared" si="0"/>
         <v>19278385.982599996</v>
       </c>
-      <c r="D14" s="143">
+      <c r="D14" s="157">
         <f t="shared" si="1"/>
         <v>11440</v>
       </c>
-      <c r="E14" s="144">
+      <c r="E14" s="158">
         <v>909</v>
       </c>
-      <c r="F14" s="144">
+      <c r="F14" s="158">
         <v>681</v>
       </c>
-      <c r="G14" s="144">
+      <c r="G14" s="158">
         <v>681</v>
       </c>
-      <c r="H14" s="144">
+      <c r="H14" s="158">
         <v>113</v>
       </c>
-      <c r="I14" s="144">
+      <c r="I14" s="158">
         <v>341</v>
       </c>
-      <c r="J14" s="144">
+      <c r="J14" s="158">
         <v>510</v>
       </c>
-      <c r="K14" s="144">
+      <c r="K14" s="158">
         <v>794</v>
       </c>
-      <c r="L14" s="144">
+      <c r="L14" s="158">
         <v>852</v>
       </c>
-      <c r="M14" s="144">
+      <c r="M14" s="158">
         <v>681</v>
       </c>
-      <c r="N14" s="144">
+      <c r="N14" s="158">
         <v>567</v>
       </c>
-      <c r="O14" s="144">
+      <c r="O14" s="158">
         <v>567</v>
       </c>
-      <c r="P14" s="144">
+      <c r="P14" s="158">
         <v>341</v>
       </c>
-      <c r="Q14" s="144">
+      <c r="Q14" s="158">
         <v>428</v>
       </c>
-      <c r="R14" s="144">
+      <c r="R14" s="158">
         <v>713</v>
       </c>
-      <c r="S14" s="144">
+      <c r="S14" s="158">
         <v>285</v>
       </c>
-      <c r="T14" s="144">
+      <c r="T14" s="158">
         <v>856</v>
       </c>
-      <c r="U14" s="144">
+      <c r="U14" s="158">
         <v>143</v>
       </c>
-      <c r="V14" s="144">
+      <c r="V14" s="158">
         <v>357</v>
       </c>
-      <c r="W14" s="144">
+      <c r="W14" s="158">
         <v>113</v>
       </c>
-      <c r="X14" s="144">
+      <c r="X14" s="158">
         <v>13</v>
       </c>
-      <c r="Y14" s="144">
+      <c r="Y14" s="158">
         <v>170</v>
       </c>
-      <c r="Z14" s="144">
+      <c r="Z14" s="158">
         <v>113</v>
       </c>
-      <c r="AA14" s="144">
+      <c r="AA14" s="158">
         <v>80</v>
       </c>
-      <c r="AB14" s="144">
+      <c r="AB14" s="158">
         <v>42</v>
       </c>
-      <c r="AC14" s="144">
+      <c r="AC14" s="158">
         <v>127</v>
       </c>
-      <c r="AD14" s="144">
+      <c r="AD14" s="158">
         <v>85</v>
       </c>
-      <c r="AE14" s="144">
+      <c r="AE14" s="158">
         <v>272</v>
       </c>
-      <c r="AF14" s="144">
+      <c r="AF14" s="158">
         <v>226</v>
       </c>
-      <c r="AG14" s="144">
+      <c r="AG14" s="158">
         <v>31</v>
       </c>
-      <c r="AH14" s="144">
+      <c r="AH14" s="158">
         <v>81</v>
       </c>
-      <c r="AI14" s="144">
+      <c r="AI14" s="158">
         <v>134</v>
       </c>
-      <c r="AJ14" s="144">
+      <c r="AJ14" s="158">
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:36" s="165" customFormat="1">
+      <c r="A15" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="163">
         <f t="shared" si="0"/>
         <v>10967014.441</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="163">
         <f t="shared" si="1"/>
         <v>7151</v>
       </c>
-      <c r="E15" s="140">
+      <c r="E15" s="164">
         <v>634</v>
       </c>
-      <c r="F15" s="140">
+      <c r="F15" s="164">
         <v>475</v>
       </c>
-      <c r="G15" s="140">
+      <c r="G15" s="164">
         <v>475</v>
       </c>
-      <c r="H15" s="140">
+      <c r="H15" s="164">
         <v>79</v>
       </c>
-      <c r="I15" s="140">
+      <c r="I15" s="164">
         <v>238</v>
       </c>
-      <c r="J15" s="140">
+      <c r="J15" s="164">
         <v>357</v>
       </c>
-      <c r="K15" s="140">
+      <c r="K15" s="164">
         <v>555</v>
       </c>
-      <c r="L15" s="140">
+      <c r="L15" s="164">
         <v>594</v>
       </c>
-      <c r="M15" s="140">
+      <c r="M15" s="164">
         <v>475</v>
       </c>
-      <c r="N15" s="140">
+      <c r="N15" s="164">
         <v>396</v>
       </c>
-      <c r="O15" s="140">
+      <c r="O15" s="164">
         <v>396</v>
       </c>
-      <c r="P15" s="140">
+      <c r="P15" s="164">
         <v>238</v>
       </c>
-      <c r="Q15" s="140">
+      <c r="Q15" s="164">
         <v>212</v>
       </c>
-      <c r="R15" s="140">
+      <c r="R15" s="164">
         <v>354</v>
       </c>
-      <c r="S15" s="140">
+      <c r="S15" s="164">
         <v>141</v>
       </c>
-      <c r="T15" s="140">
+      <c r="T15" s="164">
         <v>424</v>
       </c>
-      <c r="U15" s="140">
+      <c r="U15" s="164">
         <v>71</v>
       </c>
-      <c r="V15" s="140">
+      <c r="V15" s="164">
         <v>177</v>
       </c>
-      <c r="W15" s="140">
+      <c r="W15" s="164">
         <v>71</v>
       </c>
-      <c r="X15" s="140">
+      <c r="X15" s="164">
         <v>8</v>
       </c>
-      <c r="Y15" s="140">
+      <c r="Y15" s="164">
         <v>105</v>
       </c>
-      <c r="Z15" s="140">
+      <c r="Z15" s="164">
         <v>71</v>
       </c>
-      <c r="AA15" s="140">
+      <c r="AA15" s="164">
         <v>49</v>
       </c>
-      <c r="AB15" s="140">
+      <c r="AB15" s="164">
         <v>26</v>
       </c>
-      <c r="AC15" s="140">
+      <c r="AC15" s="164">
         <v>78</v>
       </c>
-      <c r="AD15" s="140">
+      <c r="AD15" s="164">
         <v>57</v>
       </c>
-      <c r="AE15" s="140">
+      <c r="AE15" s="164">
         <v>112</v>
       </c>
-      <c r="AF15" s="140">
+      <c r="AF15" s="164">
         <v>89</v>
       </c>
-      <c r="AG15" s="140">
+      <c r="AG15" s="164">
         <v>12</v>
       </c>
-      <c r="AH15" s="140">
+      <c r="AH15" s="164">
         <v>44</v>
       </c>
-      <c r="AI15" s="140">
+      <c r="AI15" s="164">
         <v>69</v>
       </c>
-      <c r="AJ15" s="140">
+      <c r="AJ15" s="164">
         <v>69</v>
       </c>
     </row>
@@ -3753,7 +3770,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:37">
       <c r="A17" s="13" t="s">
         <v>40</v>
       </c>
@@ -3865,7 +3882,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:37">
       <c r="A18" s="13" t="s">
         <v>41</v>
       </c>
@@ -3977,7 +3994,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:37">
       <c r="A19" s="13" t="s">
         <v>42</v>
       </c>
@@ -4089,7 +4106,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:37">
       <c r="A20" s="13" t="s">
         <v>43</v>
       </c>
@@ -4201,11 +4218,11 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
-      <c r="A21" s="147" t="s">
+    <row r="21" spans="1:37">
+      <c r="A21" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="147"/>
+      <c r="B21" s="142"/>
       <c r="C21" s="14">
         <f t="shared" si="0"/>
         <v>202837942.18770003</v>
@@ -4341,6 +4358,143 @@
       <c r="AJ21" s="14">
         <f t="shared" si="2"/>
         <v>1241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="AK23" s="160"/>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="E24" s="3">
+        <f>E14*E2</f>
+        <v>656116.19999999995</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" ref="F24:AK24" si="3">F14*F2</f>
+        <v>504517.14749999996</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="3"/>
+        <v>518171.19750000001</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="3"/>
+        <v>90286.152499999997</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="3"/>
+        <v>305616.13500000001</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="3"/>
+        <v>457591.125</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="3"/>
+        <v>720366.42500000005</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="3"/>
+        <v>780674.82</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="3"/>
+        <v>638326.83750000002</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="3"/>
+        <v>536017.70250000001</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" si="3"/>
+        <v>558754.40249999997</v>
+      </c>
+      <c r="P24" s="3">
+        <f t="shared" si="3"/>
+        <v>339117.68</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="3"/>
+        <v>446232.8</v>
+      </c>
+      <c r="R24" s="3">
+        <f t="shared" si="3"/>
+        <v>750521.625</v>
+      </c>
+      <c r="S24" s="3">
+        <f t="shared" si="3"/>
+        <v>322283.69999999995</v>
+      </c>
+      <c r="T24" s="3">
+        <f t="shared" si="3"/>
+        <v>976563.32000000007</v>
+      </c>
+      <c r="U24" s="3">
+        <f t="shared" si="3"/>
+        <v>165864.6275</v>
+      </c>
+      <c r="V24" s="3">
+        <f t="shared" si="3"/>
+        <v>424460.50499999995</v>
+      </c>
+      <c r="W24" s="3">
+        <f t="shared" si="3"/>
+        <v>400972.58999999997</v>
+      </c>
+      <c r="X24" s="3">
+        <f t="shared" si="3"/>
+        <v>47034.292500000003</v>
+      </c>
+      <c r="Y24" s="3">
+        <f t="shared" si="3"/>
+        <v>671054.6</v>
+      </c>
+      <c r="Z24" s="3">
+        <f t="shared" si="3"/>
+        <v>457040.93</v>
+      </c>
+      <c r="AA24" s="3">
+        <f t="shared" si="3"/>
+        <v>389324.76</v>
+      </c>
+      <c r="AB24" s="3">
+        <f t="shared" si="3"/>
+        <v>226076.99940000003</v>
+      </c>
+      <c r="AC24" s="3">
+        <f t="shared" si="3"/>
+        <v>726935.3</v>
+      </c>
+      <c r="AD24" s="3">
+        <f t="shared" si="3"/>
+        <v>492443.03750000003</v>
+      </c>
+      <c r="AE24" s="3">
+        <f t="shared" si="3"/>
+        <v>1746240</v>
+      </c>
+      <c r="AF24" s="3">
+        <f t="shared" si="3"/>
+        <v>1716026.0682000001</v>
+      </c>
+      <c r="AG24" s="3">
+        <f t="shared" si="3"/>
+        <v>238457.6575</v>
+      </c>
+      <c r="AH24" s="3">
+        <f t="shared" si="3"/>
+        <v>656278.60499999998</v>
+      </c>
+      <c r="AI24" s="3">
+        <f t="shared" si="3"/>
+        <v>1104102.3799999999</v>
+      </c>
+      <c r="AJ24" s="3">
+        <f t="shared" si="3"/>
+        <v>1214916.3600000001</v>
+      </c>
+      <c r="AK24" s="166">
+        <f>SUM(W24:AJ24)</f>
+        <v>10086903.5801</v>
       </c>
     </row>
   </sheetData>
@@ -4358,7 +4512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -4402,7 +4556,7 @@
     <col min="37" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15">
+    <row r="1" spans="1:36" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>249</v>
       </c>
@@ -4515,7 +4669,7 @@
       </c>
     </row>
     <row r="3" spans="1:36" s="10" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="141" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -6529,10 +6683,10 @@
       </c>
     </row>
     <row r="21" spans="1:36">
-      <c r="A21" s="147" t="s">
+      <c r="A21" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="147"/>
+      <c r="B21" s="142"/>
       <c r="C21" s="14">
         <f t="shared" si="0"/>
         <v>207989234</v>
@@ -6685,7 +6839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6712,7 +6866,7 @@
     <col min="37" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15">
+    <row r="1" spans="1:36" ht="14.25">
       <c r="A1" s="1" t="s">
         <v>250</v>
       </c>
@@ -6825,7 +6979,7 @@
       </c>
     </row>
     <row r="3" spans="1:36" s="10" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="141" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -7799,10 +7953,10 @@
       </c>
     </row>
     <row r="10" spans="1:36">
-      <c r="A10" s="147" t="s">
+      <c r="A10" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="147"/>
+      <c r="B10" s="142"/>
       <c r="C10" s="14">
         <f t="shared" si="0"/>
         <v>207989234</v>
@@ -7949,10 +8103,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AW109"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -7983,25 +8137,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="12.75">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="151" t="s">
+      <c r="B1" s="146" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="146" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="151" t="s">
+      <c r="D1" s="146" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="153" t="s">
+      <c r="E1" s="148" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="148" t="s">
+      <c r="F1" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="148" t="s">
+      <c r="G1" s="143" t="s">
         <v>50</v>
       </c>
       <c r="H1" s="6">
@@ -8102,13 +8256,13 @@
       </c>
     </row>
     <row r="2" spans="1:49" ht="12.75">
-      <c r="A2" s="150"/>
-      <c r="B2" s="152"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="148"/>
+      <c r="A2" s="145"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
@@ -19181,7 +19335,7 @@
       <c r="AV89" s="73"/>
       <c r="AW89" s="73"/>
     </row>
-    <row r="90" spans="1:49" ht="24">
+    <row r="90" spans="1:49" ht="22.5">
       <c r="A90" s="114" t="s">
         <v>155</v>
       </c>
@@ -19302,7 +19456,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:49" ht="24">
+    <row r="91" spans="1:49" ht="22.5">
       <c r="A91" s="114" t="s">
         <v>155</v>
       </c>
@@ -19423,7 +19577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:49" ht="24">
+    <row r="92" spans="1:49" ht="22.5">
       <c r="A92" s="114" t="s">
         <v>155</v>
       </c>
@@ -19544,7 +19698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:49" ht="24">
+    <row r="93" spans="1:49" ht="22.5">
       <c r="A93" s="114" t="s">
         <v>155</v>
       </c>
@@ -21772,10 +21926,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN108"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -21816,25 +21970,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="150" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="157" t="s">
+      <c r="B1" s="152" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="157" t="s">
+      <c r="C1" s="152" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="157" t="s">
+      <c r="D1" s="152" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="159" t="s">
+      <c r="E1" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="154" t="s">
+      <c r="F1" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="154" t="s">
+      <c r="G1" s="149" t="s">
         <v>50</v>
       </c>
       <c r="H1" s="16">
@@ -21935,13 +22089,13 @@
       </c>
     </row>
     <row r="2" spans="1:39">
-      <c r="A2" s="156"/>
-      <c r="B2" s="158"/>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="159"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
+      <c r="A2" s="151"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>

</xml_diff>